<commit_message>
add test for manual move
</commit_message>
<xml_diff>
--- a/SolenoidStroke-L.xlsx
+++ b/SolenoidStroke-L.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akita\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akita\Documents\GitHub\SolenoidStrokeMeasureControl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50870B56-9334-4F9B-B3CC-353B8A6D6594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1FDA5C-4AD6-473E-BCE9-C5DBACE98102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6750" yWindow="0" windowWidth="12450" windowHeight="15015" xr2:uid="{B1706589-9860-44C4-BBFB-4231996CE092}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{B1706589-9860-44C4-BBFB-4231996CE092}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -213,6 +213,50 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="ja-JP"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$7</c:f>
@@ -418,7 +462,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$2:$B$7</c15:sqref>
@@ -451,7 +495,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$D$2:$D$7</c15:sqref>
@@ -483,7 +527,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-1380-4C72-BFF7-D053262AD081}"/>
                   </c:ext>
@@ -520,7 +564,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$2:$B$7</c15:sqref>
@@ -553,7 +597,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$E$2:$E$7</c15:sqref>
@@ -585,7 +629,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-1380-4C72-BFF7-D053262AD081}"/>
                   </c:ext>
@@ -616,6 +660,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP"/>
+                  <a:t>Stroke[mm]</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ja-JP"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -678,6 +778,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP"/>
+                  <a:t>L[mH]</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ja-JP"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -727,37 +888,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="ja-JP"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1749,7 +1879,7 @@
         <v>4.55</v>
       </c>
       <c r="B2">
-        <f>A2-A$7</f>
+        <f t="shared" ref="B2:B7" si="0">A2-A$7</f>
         <v>4.0999999999999996</v>
       </c>
       <c r="C2">
@@ -1770,7 +1900,7 @@
         <v>3.5</v>
       </c>
       <c r="B3">
-        <f>A3-A$7</f>
+        <f t="shared" si="0"/>
         <v>3.05</v>
       </c>
       <c r="C3">
@@ -1791,7 +1921,7 @@
         <v>2.97</v>
       </c>
       <c r="B4">
-        <f>A4-A$7</f>
+        <f t="shared" si="0"/>
         <v>2.52</v>
       </c>
       <c r="C4">
@@ -1812,7 +1942,7 @@
         <v>1.6</v>
       </c>
       <c r="B5">
-        <f>A5-A$7</f>
+        <f t="shared" si="0"/>
         <v>1.1500000000000001</v>
       </c>
       <c r="C5">
@@ -1833,7 +1963,7 @@
         <v>0.8</v>
       </c>
       <c r="B6">
-        <f>A6-A$7</f>
+        <f t="shared" si="0"/>
         <v>0.35000000000000003</v>
       </c>
       <c r="C6">
@@ -1854,7 +1984,7 @@
         <v>0.45</v>
       </c>
       <c r="B7">
-        <f>A7-A$7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C7">

</xml_diff>